<commit_message>
DW01 - Add Customer's Request
</commit_message>
<xml_diff>
--- a/BIOS_CUSTOM/DWI-AH810-R10测试问题汇总.xlsx
+++ b/BIOS_CUSTOM/DWI-AH810-R10测试问题汇总.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raywu\Downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="120" windowWidth="23655" windowHeight="9570"/>
   </bookViews>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="50">
   <si>
     <t>BIOS版本：</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -84,7 +89,7 @@
       <rPr>
         <sz val="9"/>
         <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
+        <rFont val="新細明體"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -95,7 +100,7 @@
       <rPr>
         <sz val="9"/>
         <color theme="1"/>
-        <rFont val="宋体"/>
+        <rFont val="新細明體"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -112,7 +117,7 @@
       <rPr>
         <sz val="9"/>
         <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
+        <rFont val="新細明體"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -123,7 +128,7 @@
       <rPr>
         <sz val="9"/>
         <color theme="1"/>
-        <rFont val="宋体"/>
+        <rFont val="新細明體"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -135,7 +140,7 @@
         <b/>
         <sz val="9"/>
         <color theme="1"/>
-        <rFont val="宋体"/>
+        <rFont val="新細明體"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -146,7 +151,7 @@
       <rPr>
         <sz val="9"/>
         <color theme="1"/>
-        <rFont val="宋体"/>
+        <rFont val="新細明體"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -165,7 +170,7 @@
         <b/>
         <sz val="9"/>
         <color theme="1"/>
-        <rFont val="宋体"/>
+        <rFont val="新細明體"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -176,7 +181,7 @@
       <rPr>
         <sz val="9"/>
         <color theme="1"/>
-        <rFont val="宋体"/>
+        <rFont val="新細明體"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -188,7 +193,7 @@
         <b/>
         <sz val="9"/>
         <color theme="1"/>
-        <rFont val="宋体"/>
+        <rFont val="新細明體"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -199,7 +204,7 @@
       <rPr>
         <sz val="9"/>
         <color theme="1"/>
-        <rFont val="宋体"/>
+        <rFont val="新細明體"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -211,7 +216,7 @@
       <rPr>
         <sz val="9"/>
         <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
+        <rFont val="新細明體"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -222,7 +227,7 @@
       <rPr>
         <sz val="9"/>
         <color theme="1"/>
-        <rFont val="宋体"/>
+        <rFont val="新細明體"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -234,7 +239,7 @@
       <rPr>
         <sz val="9"/>
         <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
+        <rFont val="新細明體"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -245,7 +250,7 @@
       <rPr>
         <sz val="9"/>
         <color theme="1"/>
-        <rFont val="宋体"/>
+        <rFont val="新細明體"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -257,7 +262,7 @@
       <rPr>
         <sz val="9"/>
         <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
+        <rFont val="新細明體"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -268,7 +273,7 @@
     <r>
       <rPr>
         <sz val="9"/>
-        <rFont val="宋体"/>
+        <rFont val="新細明體"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -285,7 +290,7 @@
       <rPr>
         <sz val="9"/>
         <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
+        <rFont val="新細明體"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -296,7 +301,7 @@
       <rPr>
         <sz val="9"/>
         <color theme="1"/>
-        <rFont val="宋体"/>
+        <rFont val="新細明體"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -307,7 +312,7 @@
       <rPr>
         <sz val="9"/>
         <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
+        <rFont val="新細明體"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -318,7 +323,7 @@
       <rPr>
         <sz val="9"/>
         <color theme="1"/>
-        <rFont val="宋体"/>
+        <rFont val="新細明體"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -336,7 +341,7 @@
       <rPr>
         <sz val="9"/>
         <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
+        <rFont val="新細明體"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -347,7 +352,7 @@
       <rPr>
         <sz val="9"/>
         <color theme="1"/>
-        <rFont val="宋体"/>
+        <rFont val="新細明體"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -358,7 +363,7 @@
       <rPr>
         <sz val="9"/>
         <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
+        <rFont val="新細明體"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -369,7 +374,7 @@
       <rPr>
         <sz val="9"/>
         <color theme="1"/>
-        <rFont val="宋体"/>
+        <rFont val="新細明體"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -433,7 +438,7 @@
         <b/>
         <sz val="12"/>
         <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
+        <rFont val="新細明體"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -444,7 +449,7 @@
       <rPr>
         <sz val="9"/>
         <color theme="1"/>
-        <rFont val="宋体"/>
+        <rFont val="新細明體"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -455,7 +460,7 @@
       <rPr>
         <sz val="9"/>
         <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
+        <rFont val="新細明體"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -466,7 +471,7 @@
       <rPr>
         <sz val="9"/>
         <color theme="1"/>
-        <rFont val="宋体"/>
+        <rFont val="新細明體"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -483,7 +488,7 @@
       <rPr>
         <sz val="9"/>
         <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
+        <rFont val="新細明體"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -494,7 +499,7 @@
       <rPr>
         <sz val="9"/>
         <color theme="1"/>
-        <rFont val="宋体"/>
+        <rFont val="新細明體"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -505,7 +510,7 @@
       <rPr>
         <sz val="9"/>
         <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
+        <rFont val="新細明體"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -516,7 +521,7 @@
       <rPr>
         <sz val="9"/>
         <color theme="1"/>
-        <rFont val="宋体"/>
+        <rFont val="新細明體"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -533,7 +538,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
+        <rFont val="新細明體"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -550,7 +555,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
+        <rFont val="新細明體"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -567,7 +572,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
+        <rFont val="新細明體"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -578,7 +583,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="宋体"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -595,7 +600,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
+        <rFont val="新細明體"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -606,7 +611,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="宋体"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -617,7 +622,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
+        <rFont val="新細明體"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -628,32 +633,90 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="宋体"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t>， 即此时仅能从HDD引导，不能从U盘、光驱等设备进行引导（当设为disabled时则不再受限。）</t>
     </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>在BIOS SETUP首页，Main-&gt;Brand String，CPU信息显示不完整，可以换行显示。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>增加RTC wake up 定时开机功能</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>增加PXE网络引导启动功能：
+show出Launch PXE OpRom项（默认Disabled）
+在boot菜单中，提供network启动项。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">在chipset--usb configuration中的XHCI mode项默认为Manual.此时，将所有的USB2.0 route到EHCI, USB3.0 route到XHCI。 同时，在该页面增加十个USB开关项，可以用来控制某个USB接口的打开和关闭。
+即增加USB#1至USB#10的开关项, 值为Enabled/Disabled，默认为Enabled.
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>客户反映开机时几乎看不到GRG LOGO，请在此画面上多延迟1秒</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>当前两个VGA接口，在BIOS SETUP阶段同步复制显示；
+进入DOS下，请默认从上面的VGA接口输出（DP转的这个）。
+Graphics configuration中关闭不必要的项，仅保留右图中所示的项目</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>客户要求LOGO要满屏显示，若需要800*600分辨率的LOGO，请参考附件</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>请将Restore AC Power Loss默认为Power On</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>主板上的两个USB3.0接口中复用的USB2.0 pins ,请Route to XHCI.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>win7系统右下角声音图标在未接入耳机/speaker时会出现红叉，这是OS自动侦测的。在BIOS端能否做到不去侦测耳机插入（或始终认为有耳机），即实现不插入耳机也不会出现红叉</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Only Boot HDD选项由Enable改为Disabled后，发现Boot Option #2/#3不会立即显示，需保存退出重新进BIOS才可看到Boot Option #2/#3，要求做到随动，反之亦然</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>当前显示上的默认设置是OK的，但能否把Secondary IGFX Boot Display重新SHOW出来，以便客户在必要时还能自行设置，实现通过下面的VGA接口输出DOS界面？</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>机器在启动过程中，可以会出现在LOGO住HANG住的情形（比如右下角出现A2代码），此类现象能否让BIOS重启一次？（只需一次）</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="12">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="宋体"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -662,7 +725,7 @@
       <b/>
       <sz val="20"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="新細明體"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -670,7 +733,7 @@
     <font>
       <sz val="9"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="新細明體"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -678,7 +741,7 @@
     <font>
       <sz val="9"/>
       <color rgb="FFFF0000"/>
-      <name val="宋体"/>
+      <name val="新細明體"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -687,14 +750,14 @@
       <b/>
       <sz val="9"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="新細明體"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="宋体"/>
+      <name val="新細明體"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -703,7 +766,7 @@
       <strike/>
       <sz val="9"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -712,7 +775,7 @@
       <strike/>
       <sz val="9"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="新細明體"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -720,7 +783,7 @@
     <font>
       <sz val="9"/>
       <color rgb="FF00B050"/>
-      <name val="宋体"/>
+      <name val="新細明體"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -729,7 +792,7 @@
       <b/>
       <sz val="12"/>
       <color rgb="FFFF0000"/>
-      <name val="宋体"/>
+      <name val="新細明體"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -737,7 +800,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="宋体"/>
+      <name val="新細明體"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -764,13 +827,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.59999389629810485"/>
+        <fgColor theme="6" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.59999389629810485"/>
+        <fgColor theme="8" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -804,7 +867,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -835,34 +898,28 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="7" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="8" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -883,33 +940,50 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="一般" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1150,11 +1224,298 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>66464</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>525963</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>676486</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>1990725</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="5971964" y="23043063"/>
+          <a:ext cx="3334172" cy="2055312"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>177668</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>509019</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>1929383</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="9493118" y="23026119"/>
+          <a:ext cx="3289432" cy="2010914"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>9526</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>85726</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>266701</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>10573</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="6600826" y="21259801"/>
+          <a:ext cx="1257300" cy="905922"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>638175</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>2152650</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1028" name="Picture 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="5905500" y="24403050"/>
+          <a:ext cx="5419725" cy="2152650"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>219076</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>47626</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>2158614</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1029" name="Picture 5"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="11591926" y="25212675"/>
+          <a:ext cx="3943350" cy="2158614"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>257175</xdr:colOff>
+          <xdr:row>32</xdr:row>
+          <xdr:rowOff>104775</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>333375</xdr:colOff>
+          <xdr:row>32</xdr:row>
+          <xdr:rowOff>638175</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="7" name="Object 2" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1026"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
 </xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 佈景主題">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1196,7 +1557,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1228,9 +1589,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1262,6 +1624,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1437,50 +1800,50 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.75" style="1" customWidth="1"/>
-    <col min="2" max="2" width="14.375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="52.375" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="52.42578125" customWidth="1"/>
     <col min="4" max="4" width="9" style="1"/>
-    <col min="5" max="5" width="13.125" customWidth="1"/>
-    <col min="6" max="6" width="13.625" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
     </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="10"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="33"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>12</v>
       </c>
@@ -1496,7 +1859,7 @@
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>0</v>
       </c>
@@ -1512,7 +1875,7 @@
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>2</v>
       </c>
@@ -1528,7 +1891,7 @@
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
       <c r="B6" s="5"/>
       <c r="C6" s="2"/>
@@ -1540,7 +1903,7 @@
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
     </row>
-    <row r="7" spans="1:10" ht="30" customHeight="1">
+    <row r="7" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>4</v>
       </c>
@@ -1568,161 +1931,161 @@
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
     </row>
-    <row r="8" spans="1:10" ht="30" customHeight="1">
-      <c r="A8" s="12">
+    <row r="8" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="10">
         <v>1</v>
       </c>
-      <c r="B8" s="13">
+      <c r="B8" s="11">
         <v>43271</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="C8" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="15" t="s">
+      <c r="D8" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="16"/>
-      <c r="H8" s="17" t="s">
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="15" t="s">
         <v>28</v>
       </c>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
     </row>
-    <row r="9" spans="1:10" ht="30" customHeight="1">
-      <c r="A9" s="15">
+    <row r="9" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="13">
         <v>2</v>
       </c>
-      <c r="B9" s="18">
+      <c r="B9" s="16">
         <v>43271</v>
       </c>
-      <c r="C9" s="19" t="s">
+      <c r="C9" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="15" t="s">
+      <c r="D9" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="17" t="s">
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="15" t="s">
         <v>28</v>
       </c>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
     </row>
-    <row r="10" spans="1:10" ht="30" customHeight="1">
-      <c r="A10" s="15">
+    <row r="10" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="13">
         <v>3</v>
       </c>
-      <c r="B10" s="18">
+      <c r="B10" s="16">
         <v>43271</v>
       </c>
-      <c r="C10" s="19" t="s">
+      <c r="C10" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="D10" s="15" t="s">
+      <c r="D10" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="16"/>
-      <c r="H10" s="17" t="s">
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="15" t="s">
         <v>28</v>
       </c>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
     </row>
-    <row r="11" spans="1:10" ht="30" customHeight="1">
-      <c r="A11" s="15">
+    <row r="11" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="13">
         <v>4</v>
       </c>
-      <c r="B11" s="18">
+      <c r="B11" s="16">
         <v>43271</v>
       </c>
-      <c r="C11" s="19" t="s">
+      <c r="C11" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="D11" s="15" t="s">
+      <c r="D11" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="16"/>
-      <c r="H11" s="17" t="s">
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="15" t="s">
         <v>28</v>
       </c>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
     </row>
-    <row r="12" spans="1:10" ht="30" customHeight="1">
-      <c r="A12" s="15">
+    <row r="12" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="13">
         <v>6</v>
       </c>
-      <c r="B12" s="18">
+      <c r="B12" s="16">
         <v>43271</v>
       </c>
-      <c r="C12" s="19" t="s">
+      <c r="C12" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="15" t="s">
+      <c r="D12" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
-      <c r="G12" s="16"/>
-      <c r="H12" s="17" t="s">
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="15" t="s">
         <v>28</v>
       </c>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
     </row>
-    <row r="13" spans="1:10" ht="30" customHeight="1">
-      <c r="A13" s="15">
+    <row r="13" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="13">
         <v>7</v>
       </c>
-      <c r="B13" s="18">
+      <c r="B13" s="16">
         <v>43278</v>
       </c>
-      <c r="C13" s="19" t="s">
+      <c r="C13" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="D13" s="15" t="s">
+      <c r="D13" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="E13" s="16"/>
-      <c r="F13" s="16"/>
-      <c r="G13" s="16"/>
-      <c r="H13" s="17" t="s">
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="15" t="s">
         <v>28</v>
       </c>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
     </row>
-    <row r="14" spans="1:10" ht="30" customHeight="1">
-      <c r="A14" s="15">
+    <row r="14" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="13">
         <v>8</v>
       </c>
-      <c r="B14" s="18">
+      <c r="B14" s="16">
         <v>43278</v>
       </c>
-      <c r="C14" s="19" t="s">
+      <c r="C14" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="D14" s="15" t="s">
+      <c r="D14" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="E14" s="16"/>
-      <c r="F14" s="16"/>
-      <c r="G14" s="16"/>
-      <c r="H14" s="17" t="s">
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="15" t="s">
         <v>28</v>
       </c>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
     </row>
-    <row r="15" spans="1:10" ht="30" customHeight="1">
+    <row r="15" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="7">
         <v>9</v>
       </c>
@@ -1740,7 +2103,7 @@
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
     </row>
-    <row r="16" spans="1:10" ht="125.25" customHeight="1">
+    <row r="16" spans="1:10" ht="125.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="7">
         <v>10</v>
       </c>
@@ -1756,7 +2119,7 @@
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
     </row>
-    <row r="17" spans="1:10" ht="158.25" customHeight="1">
+    <row r="17" spans="1:10" ht="158.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
         <v>11</v>
       </c>
@@ -1772,7 +2135,7 @@
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
     </row>
-    <row r="18" spans="1:10" ht="162" customHeight="1">
+    <row r="18" spans="1:10" ht="162" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="7">
         <v>12</v>
       </c>
@@ -1788,7 +2151,7 @@
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
     </row>
-    <row r="19" spans="1:10" ht="255" customHeight="1">
+    <row r="19" spans="1:10" ht="255" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="7">
         <v>13</v>
       </c>
@@ -1804,7 +2167,7 @@
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
     </row>
-    <row r="20" spans="1:10" ht="198.75" customHeight="1">
+    <row r="20" spans="1:10" ht="198.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="7">
         <v>14</v>
       </c>
@@ -1820,265 +2183,277 @@
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
     </row>
-    <row r="21" spans="1:10" s="28" customFormat="1" ht="75.75" customHeight="1">
-      <c r="A21" s="26">
+    <row r="21" spans="1:10" s="21" customFormat="1" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="20">
         <v>15</v>
       </c>
-      <c r="B21" s="26"/>
-      <c r="C21" s="27" t="s">
+      <c r="B21" s="20"/>
+      <c r="C21" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="D21" s="26"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
-      <c r="G21" s="11"/>
-      <c r="H21" s="11"/>
-    </row>
-    <row r="22" spans="1:10" s="28" customFormat="1" ht="63.75" customHeight="1">
-      <c r="A22" s="26">
+      <c r="D21" s="20"/>
+      <c r="E21" s="27"/>
+      <c r="F21" s="27"/>
+      <c r="G21" s="27"/>
+      <c r="H21" s="27"/>
+    </row>
+    <row r="22" spans="1:10" s="21" customFormat="1" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="20">
         <v>16</v>
       </c>
-      <c r="B22" s="26"/>
-      <c r="C22" s="27" t="s">
+      <c r="B22" s="20"/>
+      <c r="C22" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="D22" s="26"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="11"/>
-      <c r="G22" s="11"/>
-      <c r="H22" s="11"/>
-    </row>
-    <row r="23" spans="1:10" s="28" customFormat="1" ht="51" customHeight="1">
-      <c r="A23" s="26">
+      <c r="D22" s="20"/>
+      <c r="E22" s="27"/>
+      <c r="F22" s="27"/>
+      <c r="G22" s="27"/>
+      <c r="H22" s="27"/>
+    </row>
+    <row r="23" spans="1:10" s="21" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="20">
         <v>17</v>
       </c>
-      <c r="B23" s="29"/>
-      <c r="C23" s="31" t="s">
+      <c r="B23" s="22"/>
+      <c r="C23" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="D23" s="29"/>
-      <c r="E23" s="30"/>
-      <c r="F23" s="30"/>
-      <c r="G23" s="30"/>
-      <c r="H23" s="30"/>
-    </row>
-    <row r="24" spans="1:10" s="28" customFormat="1" ht="45.75" customHeight="1">
-      <c r="A24" s="26">
+      <c r="D23" s="22"/>
+      <c r="E23" s="23"/>
+      <c r="F23" s="23"/>
+      <c r="G23" s="23"/>
+      <c r="H23" s="23"/>
+    </row>
+    <row r="24" spans="1:10" s="21" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="20">
         <v>18</v>
       </c>
-      <c r="B24" s="29"/>
-      <c r="C24" s="31" t="s">
+      <c r="B24" s="22"/>
+      <c r="C24" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="D24" s="29"/>
-      <c r="E24" s="30"/>
-      <c r="F24" s="30"/>
-      <c r="G24" s="30"/>
-      <c r="H24" s="30"/>
-    </row>
-    <row r="25" spans="1:10" s="28" customFormat="1" ht="91.5" customHeight="1">
-      <c r="A25" s="26">
+      <c r="D24" s="22"/>
+      <c r="E24" s="23"/>
+      <c r="F24" s="23"/>
+      <c r="G24" s="23"/>
+      <c r="H24" s="23"/>
+    </row>
+    <row r="25" spans="1:10" s="21" customFormat="1" ht="91.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="20">
         <v>19</v>
       </c>
-      <c r="B25" s="29"/>
-      <c r="C25" s="31" t="s">
+      <c r="B25" s="22"/>
+      <c r="C25" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="D25" s="29"/>
-      <c r="E25" s="30"/>
-      <c r="F25" s="30"/>
-      <c r="G25" s="30"/>
-      <c r="H25" s="30"/>
-    </row>
-    <row r="26" spans="1:10" s="28" customFormat="1" ht="53.25" customHeight="1">
-      <c r="A26" s="26">
+      <c r="D25" s="22"/>
+      <c r="E25" s="23"/>
+      <c r="F25" s="23"/>
+      <c r="G25" s="23"/>
+      <c r="H25" s="23"/>
+    </row>
+    <row r="26" spans="1:10" s="21" customFormat="1" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="20">
         <v>20</v>
       </c>
-      <c r="B26" s="29"/>
-      <c r="C26" s="31" t="s">
+      <c r="B26" s="22"/>
+      <c r="C26" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="D26" s="29"/>
-      <c r="E26" s="30"/>
-      <c r="F26" s="30"/>
-      <c r="G26" s="30"/>
-      <c r="H26" s="30"/>
-    </row>
-    <row r="27" spans="1:10" s="23" customFormat="1">
-      <c r="A27" s="22">
+      <c r="D26" s="22"/>
+      <c r="E26" s="23"/>
+      <c r="F26" s="23"/>
+      <c r="G26" s="23"/>
+      <c r="H26" s="23"/>
+    </row>
+    <row r="27" spans="1:10" s="21" customFormat="1" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="20">
         <v>21</v>
       </c>
-      <c r="B27" s="24"/>
-      <c r="C27" s="32"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="25"/>
-      <c r="F27" s="25"/>
-      <c r="G27" s="25"/>
-      <c r="H27" s="25"/>
-    </row>
-    <row r="28" spans="1:10" s="23" customFormat="1">
-      <c r="A28" s="22">
+      <c r="B27" s="22"/>
+      <c r="C27" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="D27" s="22"/>
+      <c r="E27" s="23"/>
+      <c r="F27" s="23"/>
+      <c r="G27" s="23"/>
+      <c r="H27" s="23"/>
+    </row>
+    <row r="28" spans="1:10" s="21" customFormat="1" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="20">
         <v>22</v>
       </c>
-      <c r="B28" s="24"/>
-      <c r="C28" s="32"/>
-      <c r="D28" s="24"/>
-      <c r="E28" s="25"/>
-      <c r="F28" s="25"/>
-      <c r="G28" s="25"/>
-      <c r="H28" s="25"/>
-    </row>
-    <row r="29" spans="1:10" s="23" customFormat="1">
-      <c r="A29" s="22">
+      <c r="B28" s="22"/>
+      <c r="C28" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="D28" s="22"/>
+      <c r="E28" s="23"/>
+      <c r="F28" s="23"/>
+      <c r="G28" s="23"/>
+      <c r="H28" s="23"/>
+    </row>
+    <row r="29" spans="1:10" s="21" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="20">
         <v>23</v>
       </c>
-      <c r="B29" s="24"/>
-      <c r="C29" s="32"/>
-      <c r="D29" s="24"/>
-      <c r="E29" s="25"/>
-      <c r="F29" s="25"/>
-      <c r="G29" s="25"/>
-      <c r="H29" s="25"/>
-    </row>
-    <row r="30" spans="1:10" s="23" customFormat="1">
-      <c r="A30" s="22">
+      <c r="B29" s="22"/>
+      <c r="C29" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="D29" s="22"/>
+      <c r="E29" s="23"/>
+      <c r="F29" s="23"/>
+      <c r="G29" s="23"/>
+      <c r="H29" s="23"/>
+    </row>
+    <row r="30" spans="1:10" s="21" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="20">
         <v>24</v>
       </c>
-      <c r="B30" s="24"/>
-      <c r="C30" s="32"/>
-      <c r="D30" s="24"/>
-      <c r="E30" s="25"/>
-      <c r="F30" s="25"/>
-      <c r="G30" s="25"/>
-      <c r="H30" s="25"/>
-    </row>
-    <row r="31" spans="1:10">
+      <c r="B30" s="22"/>
+      <c r="C30" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="D30" s="22"/>
+      <c r="E30" s="23"/>
+      <c r="F30" s="23"/>
+      <c r="G30" s="23"/>
+      <c r="H30" s="23"/>
+    </row>
+    <row r="31" spans="1:10" ht="165.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="7">
         <v>25</v>
       </c>
-      <c r="B31" s="20"/>
-      <c r="C31" s="21"/>
-      <c r="D31" s="20"/>
-      <c r="E31" s="21"/>
-      <c r="F31" s="21"/>
-      <c r="G31" s="21"/>
-      <c r="H31" s="21"/>
+      <c r="B31" s="18"/>
+      <c r="C31" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="D31" s="18"/>
+      <c r="E31" s="19"/>
+      <c r="F31" s="19"/>
+      <c r="G31" s="19"/>
+      <c r="H31" s="19"/>
       <c r="I31" s="2"/>
       <c r="J31" s="2"/>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:10" ht="180.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="7">
         <v>26</v>
       </c>
-      <c r="B32" s="20"/>
-      <c r="C32" s="21"/>
-      <c r="D32" s="20"/>
-      <c r="E32" s="21"/>
-      <c r="F32" s="21"/>
-      <c r="G32" s="21"/>
-      <c r="H32" s="21"/>
+      <c r="B32" s="18"/>
+      <c r="C32" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="D32" s="18"/>
+      <c r="E32" s="19"/>
+      <c r="F32" s="19"/>
+      <c r="G32" s="19"/>
+      <c r="H32" s="19"/>
       <c r="I32" s="2"/>
       <c r="J32" s="2"/>
     </row>
-    <row r="33" spans="1:10">
-      <c r="A33" s="7">
+    <row r="33" spans="1:10" s="32" customFormat="1" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="28">
         <v>27</v>
       </c>
-      <c r="B33" s="20"/>
-      <c r="C33" s="21"/>
-      <c r="D33" s="20"/>
-      <c r="E33" s="21"/>
-      <c r="F33" s="21"/>
-      <c r="G33" s="21"/>
-      <c r="H33" s="21"/>
-      <c r="I33" s="2"/>
-      <c r="J33" s="2"/>
-    </row>
-    <row r="34" spans="1:10">
-      <c r="A34" s="7">
+      <c r="B33" s="29"/>
+      <c r="C33" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="D33" s="29"/>
+      <c r="E33" s="31"/>
+      <c r="F33" s="31"/>
+      <c r="G33" s="31"/>
+      <c r="H33" s="31"/>
+    </row>
+    <row r="34" spans="1:10" s="32" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="28">
         <v>28</v>
       </c>
-      <c r="B34" s="20"/>
-      <c r="C34" s="21"/>
-      <c r="D34" s="20"/>
-      <c r="E34" s="21"/>
-      <c r="F34" s="21"/>
-      <c r="G34" s="21"/>
-      <c r="H34" s="21"/>
-      <c r="I34" s="2"/>
-      <c r="J34" s="2"/>
-    </row>
-    <row r="35" spans="1:10">
-      <c r="A35" s="7">
+      <c r="B34" s="29"/>
+      <c r="C34" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="D34" s="29"/>
+      <c r="E34" s="31"/>
+      <c r="F34" s="31"/>
+      <c r="G34" s="31"/>
+      <c r="H34" s="31"/>
+    </row>
+    <row r="35" spans="1:10" s="32" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="28">
         <v>29</v>
       </c>
-      <c r="B35" s="20"/>
-      <c r="C35" s="21"/>
-      <c r="D35" s="20"/>
-      <c r="E35" s="21"/>
-      <c r="F35" s="21"/>
-      <c r="G35" s="21"/>
-      <c r="H35" s="21"/>
-      <c r="I35" s="2"/>
-      <c r="J35" s="2"/>
-    </row>
-    <row r="36" spans="1:10">
-      <c r="A36" s="7">
+      <c r="B35" s="29"/>
+      <c r="C35" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="D35" s="29"/>
+      <c r="E35" s="31"/>
+      <c r="F35" s="31"/>
+      <c r="G35" s="31"/>
+      <c r="H35" s="31"/>
+    </row>
+    <row r="36" spans="1:10" s="32" customFormat="1" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="28">
         <v>30</v>
       </c>
-      <c r="B36" s="20"/>
-      <c r="C36" s="21"/>
-      <c r="D36" s="20"/>
-      <c r="E36" s="21"/>
-      <c r="F36" s="21"/>
-      <c r="G36" s="21"/>
-      <c r="H36" s="21"/>
-      <c r="I36" s="2"/>
-      <c r="J36" s="2"/>
-    </row>
-    <row r="37" spans="1:10">
-      <c r="A37" s="7">
+      <c r="B36" s="29"/>
+      <c r="C36" s="30" t="s">
+        <v>45</v>
+      </c>
+      <c r="D36" s="29"/>
+      <c r="E36" s="31"/>
+      <c r="F36" s="31"/>
+      <c r="G36" s="31"/>
+      <c r="H36" s="31"/>
+    </row>
+    <row r="37" spans="1:10" s="32" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="28">
         <v>31</v>
       </c>
-      <c r="B37" s="20"/>
-      <c r="C37" s="21"/>
-      <c r="D37" s="20"/>
-      <c r="E37" s="21"/>
-      <c r="F37" s="21"/>
-      <c r="G37" s="21"/>
-      <c r="H37" s="21"/>
-      <c r="I37" s="2"/>
-      <c r="J37" s="2"/>
-    </row>
-    <row r="38" spans="1:10">
-      <c r="A38" s="7">
+      <c r="B37" s="29"/>
+      <c r="C37" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="D37" s="29"/>
+      <c r="E37" s="31"/>
+      <c r="F37" s="31"/>
+      <c r="G37" s="31"/>
+      <c r="H37" s="31"/>
+    </row>
+    <row r="38" spans="1:10" s="32" customFormat="1" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="28">
         <v>32</v>
       </c>
-      <c r="B38" s="20"/>
-      <c r="C38" s="21"/>
-      <c r="D38" s="20"/>
-      <c r="E38" s="21"/>
-      <c r="F38" s="21"/>
-      <c r="G38" s="21"/>
-      <c r="H38" s="21"/>
-      <c r="I38" s="2"/>
-      <c r="J38" s="2"/>
-    </row>
-    <row r="39" spans="1:10">
-      <c r="A39" s="7">
+      <c r="B38" s="29"/>
+      <c r="C38" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="D38" s="29"/>
+      <c r="E38" s="31"/>
+      <c r="F38" s="31"/>
+      <c r="G38" s="31"/>
+      <c r="H38" s="31"/>
+    </row>
+    <row r="39" spans="1:10" s="32" customFormat="1" ht="71.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="28">
         <v>33</v>
       </c>
-      <c r="B39" s="20"/>
-      <c r="C39" s="21"/>
-      <c r="D39" s="20"/>
-      <c r="E39" s="21"/>
-      <c r="F39" s="21"/>
-      <c r="G39" s="21"/>
-      <c r="H39" s="21"/>
-      <c r="I39" s="2"/>
-      <c r="J39" s="2"/>
-    </row>
-    <row r="40" spans="1:10">
+      <c r="B39" s="29"/>
+      <c r="C39" s="30" t="s">
+        <v>49</v>
+      </c>
+      <c r="D39" s="29"/>
+      <c r="E39" s="31"/>
+      <c r="F39" s="31"/>
+      <c r="G39" s="31"/>
+      <c r="H39" s="31"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="5"/>
       <c r="B40" s="5"/>
       <c r="C40" s="2"/>
@@ -2090,7 +2465,7 @@
       <c r="I40" s="2"/>
       <c r="J40" s="2"/>
     </row>
-    <row r="41" spans="1:10">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="5"/>
       <c r="B41" s="5"/>
       <c r="C41" s="2"/>
@@ -2102,7 +2477,7 @@
       <c r="I41" s="2"/>
       <c r="J41" s="2"/>
     </row>
-    <row r="42" spans="1:10">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="5"/>
       <c r="B42" s="5"/>
       <c r="C42" s="2"/>
@@ -2114,7 +2489,7 @@
       <c r="I42" s="2"/>
       <c r="J42" s="2"/>
     </row>
-    <row r="43" spans="1:10">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="5"/>
       <c r="B43" s="5"/>
       <c r="C43" s="2"/>
@@ -2126,7 +2501,7 @@
       <c r="I43" s="2"/>
       <c r="J43" s="2"/>
     </row>
-    <row r="44" spans="1:10">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="5"/>
       <c r="B44" s="5"/>
       <c r="C44" s="2"/>
@@ -2138,7 +2513,7 @@
       <c r="I44" s="2"/>
       <c r="J44" s="2"/>
     </row>
-    <row r="45" spans="1:10">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="5"/>
       <c r="B45" s="5"/>
       <c r="C45" s="2"/>
@@ -2150,7 +2525,7 @@
       <c r="I45" s="2"/>
       <c r="J45" s="2"/>
     </row>
-    <row r="46" spans="1:10">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="5"/>
       <c r="B46" s="5"/>
       <c r="C46" s="2"/>
@@ -2162,7 +2537,7 @@
       <c r="I46" s="2"/>
       <c r="J46" s="2"/>
     </row>
-    <row r="47" spans="1:10">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="5"/>
       <c r="B47" s="5"/>
       <c r="C47" s="2"/>
@@ -2174,7 +2549,7 @@
       <c r="I47" s="2"/>
       <c r="J47" s="2"/>
     </row>
-    <row r="48" spans="1:10">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="5"/>
       <c r="B48" s="5"/>
       <c r="C48" s="2"/>
@@ -2186,7 +2561,7 @@
       <c r="I48" s="2"/>
       <c r="J48" s="2"/>
     </row>
-    <row r="49" spans="1:10">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="5"/>
       <c r="B49" s="5"/>
       <c r="C49" s="2"/>
@@ -2198,7 +2573,7 @@
       <c r="I49" s="2"/>
       <c r="J49" s="2"/>
     </row>
-    <row r="50" spans="1:10">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="5"/>
       <c r="B50" s="5"/>
       <c r="C50" s="2"/>
@@ -2210,7 +2585,7 @@
       <c r="I50" s="2"/>
       <c r="J50" s="2"/>
     </row>
-    <row r="51" spans="1:10">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="5"/>
       <c r="B51" s="5"/>
       <c r="C51" s="2"/>
@@ -2222,7 +2597,7 @@
       <c r="I51" s="2"/>
       <c r="J51" s="2"/>
     </row>
-    <row r="52" spans="1:10">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="5"/>
       <c r="B52" s="5"/>
       <c r="C52" s="2"/>
@@ -2234,7 +2609,7 @@
       <c r="I52" s="2"/>
       <c r="J52" s="2"/>
     </row>
-    <row r="53" spans="1:10">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="5"/>
       <c r="B53" s="5"/>
       <c r="C53" s="2"/>
@@ -2246,7 +2621,7 @@
       <c r="I53" s="2"/>
       <c r="J53" s="2"/>
     </row>
-    <row r="54" spans="1:10">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="5"/>
       <c r="B54" s="5"/>
       <c r="C54" s="2"/>
@@ -2258,7 +2633,7 @@
       <c r="I54" s="2"/>
       <c r="J54" s="2"/>
     </row>
-    <row r="55" spans="1:10">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="5"/>
       <c r="B55" s="5"/>
       <c r="C55" s="2"/>
@@ -2270,7 +2645,7 @@
       <c r="I55" s="2"/>
       <c r="J55" s="2"/>
     </row>
-    <row r="56" spans="1:10">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="5"/>
       <c r="B56" s="5"/>
       <c r="C56" s="2"/>
@@ -2282,7 +2657,7 @@
       <c r="I56" s="2"/>
       <c r="J56" s="2"/>
     </row>
-    <row r="57" spans="1:10">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="5"/>
       <c r="B57" s="5"/>
       <c r="C57" s="2"/>
@@ -2294,7 +2669,7 @@
       <c r="I57" s="2"/>
       <c r="J57" s="2"/>
     </row>
-    <row r="58" spans="1:10">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="5"/>
       <c r="B58" s="5"/>
       <c r="C58" s="2"/>
@@ -2306,7 +2681,7 @@
       <c r="I58" s="2"/>
       <c r="J58" s="2"/>
     </row>
-    <row r="59" spans="1:10">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="5"/>
       <c r="B59" s="5"/>
       <c r="C59" s="2"/>
@@ -2318,7 +2693,7 @@
       <c r="I59" s="2"/>
       <c r="J59" s="2"/>
     </row>
-    <row r="60" spans="1:10">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="5"/>
       <c r="B60" s="5"/>
       <c r="C60" s="2"/>
@@ -2330,7 +2705,7 @@
       <c r="I60" s="2"/>
       <c r="J60" s="2"/>
     </row>
-    <row r="61" spans="1:10">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="5"/>
       <c r="B61" s="5"/>
       <c r="C61" s="2"/>
@@ -2342,7 +2717,7 @@
       <c r="I61" s="2"/>
       <c r="J61" s="2"/>
     </row>
-    <row r="62" spans="1:10">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="5"/>
       <c r="B62" s="5"/>
       <c r="C62" s="2"/>
@@ -2354,7 +2729,7 @@
       <c r="I62" s="2"/>
       <c r="J62" s="2"/>
     </row>
-    <row r="63" spans="1:10">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="5"/>
       <c r="B63" s="5"/>
       <c r="C63" s="2"/>
@@ -2366,7 +2741,7 @@
       <c r="I63" s="2"/>
       <c r="J63" s="2"/>
     </row>
-    <row r="64" spans="1:10">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="5"/>
       <c r="B64" s="5"/>
       <c r="C64" s="2"/>
@@ -2378,7 +2753,7 @@
       <c r="I64" s="2"/>
       <c r="J64" s="2"/>
     </row>
-    <row r="65" spans="1:10">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="5"/>
       <c r="B65" s="5"/>
       <c r="C65" s="2"/>
@@ -2390,7 +2765,7 @@
       <c r="I65" s="2"/>
       <c r="J65" s="2"/>
     </row>
-    <row r="66" spans="1:10">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="5"/>
       <c r="B66" s="5"/>
       <c r="C66" s="2"/>
@@ -2402,7 +2777,7 @@
       <c r="I66" s="2"/>
       <c r="J66" s="2"/>
     </row>
-    <row r="67" spans="1:10">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="5"/>
       <c r="B67" s="5"/>
       <c r="C67" s="2"/>
@@ -2414,7 +2789,7 @@
       <c r="I67" s="2"/>
       <c r="J67" s="2"/>
     </row>
-    <row r="68" spans="1:10">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="5"/>
       <c r="B68" s="5"/>
       <c r="C68" s="2"/>
@@ -2426,7 +2801,7 @@
       <c r="I68" s="2"/>
       <c r="J68" s="2"/>
     </row>
-    <row r="69" spans="1:10">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="5"/>
       <c r="B69" s="5"/>
       <c r="C69" s="2"/>
@@ -2438,7 +2813,7 @@
       <c r="I69" s="2"/>
       <c r="J69" s="2"/>
     </row>
-    <row r="70" spans="1:10">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="5"/>
       <c r="B70" s="5"/>
       <c r="C70" s="2"/>
@@ -2450,7 +2825,7 @@
       <c r="I70" s="2"/>
       <c r="J70" s="2"/>
     </row>
-    <row r="71" spans="1:10">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="5"/>
       <c r="B71" s="5"/>
       <c r="C71" s="2"/>
@@ -2462,7 +2837,7 @@
       <c r="I71" s="2"/>
       <c r="J71" s="2"/>
     </row>
-    <row r="72" spans="1:10">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="5"/>
       <c r="B72" s="5"/>
       <c r="C72" s="2"/>
@@ -2474,7 +2849,7 @@
       <c r="I72" s="2"/>
       <c r="J72" s="2"/>
     </row>
-    <row r="73" spans="1:10">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" s="5"/>
       <c r="B73" s="5"/>
       <c r="C73" s="2"/>
@@ -2486,7 +2861,7 @@
       <c r="I73" s="2"/>
       <c r="J73" s="2"/>
     </row>
-    <row r="74" spans="1:10">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" s="5"/>
       <c r="B74" s="5"/>
       <c r="C74" s="2"/>
@@ -2498,7 +2873,7 @@
       <c r="I74" s="2"/>
       <c r="J74" s="2"/>
     </row>
-    <row r="75" spans="1:10">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="5"/>
       <c r="B75" s="5"/>
       <c r="C75" s="2"/>
@@ -2510,7 +2885,7 @@
       <c r="I75" s="2"/>
       <c r="J75" s="2"/>
     </row>
-    <row r="76" spans="1:10">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" s="5"/>
       <c r="B76" s="5"/>
       <c r="C76" s="2"/>
@@ -2522,7 +2897,7 @@
       <c r="I76" s="2"/>
       <c r="J76" s="2"/>
     </row>
-    <row r="77" spans="1:10">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" s="5"/>
       <c r="B77" s="5"/>
       <c r="C77" s="2"/>
@@ -2534,7 +2909,7 @@
       <c r="I77" s="2"/>
       <c r="J77" s="2"/>
     </row>
-    <row r="78" spans="1:10">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" s="5"/>
       <c r="B78" s="5"/>
       <c r="C78" s="2"/>
@@ -2546,7 +2921,7 @@
       <c r="I78" s="2"/>
       <c r="J78" s="2"/>
     </row>
-    <row r="79" spans="1:10">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" s="5"/>
       <c r="B79" s="5"/>
       <c r="C79" s="2"/>
@@ -2558,7 +2933,7 @@
       <c r="I79" s="2"/>
       <c r="J79" s="2"/>
     </row>
-    <row r="80" spans="1:10">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" s="5"/>
       <c r="B80" s="5"/>
       <c r="C80" s="2"/>
@@ -2570,7 +2945,7 @@
       <c r="I80" s="2"/>
       <c r="J80" s="2"/>
     </row>
-    <row r="81" spans="1:10">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" s="5"/>
       <c r="B81" s="5"/>
       <c r="C81" s="2"/>
@@ -2582,7 +2957,7 @@
       <c r="I81" s="2"/>
       <c r="J81" s="2"/>
     </row>
-    <row r="82" spans="1:10">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" s="5"/>
       <c r="B82" s="5"/>
       <c r="C82" s="2"/>
@@ -2594,7 +2969,7 @@
       <c r="I82" s="2"/>
       <c r="J82" s="2"/>
     </row>
-    <row r="83" spans="1:10">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" s="5"/>
       <c r="B83" s="5"/>
       <c r="C83" s="2"/>
@@ -2606,7 +2981,7 @@
       <c r="I83" s="2"/>
       <c r="J83" s="2"/>
     </row>
-    <row r="84" spans="1:10">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" s="5"/>
       <c r="B84" s="5"/>
       <c r="C84" s="2"/>
@@ -2618,7 +2993,7 @@
       <c r="I84" s="2"/>
       <c r="J84" s="2"/>
     </row>
-    <row r="85" spans="1:10">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" s="5"/>
       <c r="B85" s="5"/>
       <c r="C85" s="2"/>
@@ -2630,7 +3005,7 @@
       <c r="I85" s="2"/>
       <c r="J85" s="2"/>
     </row>
-    <row r="86" spans="1:10">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" s="5"/>
       <c r="B86" s="5"/>
       <c r="C86" s="2"/>
@@ -2642,7 +3017,7 @@
       <c r="I86" s="2"/>
       <c r="J86" s="2"/>
     </row>
-    <row r="87" spans="1:10">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" s="5"/>
       <c r="B87" s="5"/>
       <c r="C87" s="2"/>
@@ -2654,7 +3029,7 @@
       <c r="I87" s="2"/>
       <c r="J87" s="2"/>
     </row>
-    <row r="88" spans="1:10">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" s="5"/>
       <c r="B88" s="5"/>
       <c r="C88" s="2"/>
@@ -2666,7 +3041,7 @@
       <c r="I88" s="2"/>
       <c r="J88" s="2"/>
     </row>
-    <row r="89" spans="1:10">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" s="5"/>
       <c r="B89" s="5"/>
       <c r="C89" s="2"/>
@@ -2678,7 +3053,7 @@
       <c r="I89" s="2"/>
       <c r="J89" s="2"/>
     </row>
-    <row r="90" spans="1:10">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" s="5"/>
       <c r="B90" s="5"/>
       <c r="C90" s="2"/>
@@ -2690,7 +3065,7 @@
       <c r="I90" s="2"/>
       <c r="J90" s="2"/>
     </row>
-    <row r="91" spans="1:10">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" s="5"/>
       <c r="B91" s="5"/>
       <c r="C91" s="2"/>
@@ -2702,7 +3077,7 @@
       <c r="I91" s="2"/>
       <c r="J91" s="2"/>
     </row>
-    <row r="92" spans="1:10">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" s="5"/>
       <c r="B92" s="5"/>
       <c r="C92" s="2"/>
@@ -2714,7 +3089,7 @@
       <c r="I92" s="2"/>
       <c r="J92" s="2"/>
     </row>
-    <row r="93" spans="1:10">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" s="5"/>
       <c r="B93" s="5"/>
       <c r="C93" s="2"/>
@@ -2726,7 +3101,7 @@
       <c r="I93" s="2"/>
       <c r="J93" s="2"/>
     </row>
-    <row r="94" spans="1:10">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" s="5"/>
       <c r="B94" s="5"/>
       <c r="C94" s="2"/>
@@ -2738,7 +3113,7 @@
       <c r="I94" s="2"/>
       <c r="J94" s="2"/>
     </row>
-    <row r="95" spans="1:10">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" s="5"/>
       <c r="B95" s="5"/>
       <c r="C95" s="2"/>
@@ -2750,7 +3125,7 @@
       <c r="I95" s="2"/>
       <c r="J95" s="2"/>
     </row>
-    <row r="96" spans="1:10">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" s="5"/>
       <c r="B96" s="5"/>
       <c r="C96" s="2"/>
@@ -2762,7 +3137,7 @@
       <c r="I96" s="2"/>
       <c r="J96" s="2"/>
     </row>
-    <row r="97" spans="1:10">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" s="5"/>
       <c r="B97" s="5"/>
       <c r="C97" s="2"/>
@@ -2774,7 +3149,7 @@
       <c r="I97" s="2"/>
       <c r="J97" s="2"/>
     </row>
-    <row r="98" spans="1:10">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" s="5"/>
       <c r="B98" s="5"/>
       <c r="C98" s="2"/>
@@ -2786,7 +3161,7 @@
       <c r="I98" s="2"/>
       <c r="J98" s="2"/>
     </row>
-    <row r="99" spans="1:10">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" s="5"/>
       <c r="B99" s="5"/>
       <c r="C99" s="2"/>
@@ -2798,7 +3173,7 @@
       <c r="I99" s="2"/>
       <c r="J99" s="2"/>
     </row>
-    <row r="100" spans="1:10">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" s="5"/>
       <c r="B100" s="5"/>
       <c r="C100" s="2"/>
@@ -2810,7 +3185,7 @@
       <c r="I100" s="2"/>
       <c r="J100" s="2"/>
     </row>
-    <row r="101" spans="1:10">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" s="5"/>
       <c r="B101" s="5"/>
       <c r="C101" s="2"/>
@@ -2822,7 +3197,7 @@
       <c r="I101" s="2"/>
       <c r="J101" s="2"/>
     </row>
-    <row r="102" spans="1:10">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102" s="5"/>
       <c r="B102" s="5"/>
       <c r="C102" s="2"/>
@@ -2834,7 +3209,7 @@
       <c r="I102" s="2"/>
       <c r="J102" s="2"/>
     </row>
-    <row r="103" spans="1:10">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103" s="5"/>
       <c r="B103" s="5"/>
       <c r="C103" s="2"/>
@@ -2846,7 +3221,7 @@
       <c r="I103" s="2"/>
       <c r="J103" s="2"/>
     </row>
-    <row r="104" spans="1:10">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104" s="5"/>
       <c r="B104" s="5"/>
       <c r="C104" s="2"/>
@@ -2858,7 +3233,7 @@
       <c r="I104" s="2"/>
       <c r="J104" s="2"/>
     </row>
-    <row r="105" spans="1:10">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A105" s="5"/>
       <c r="B105" s="5"/>
       <c r="C105" s="2"/>
@@ -2870,7 +3245,7 @@
       <c r="I105" s="2"/>
       <c r="J105" s="2"/>
     </row>
-    <row r="106" spans="1:10">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A106" s="5"/>
       <c r="B106" s="5"/>
       <c r="C106" s="2"/>
@@ -2882,7 +3257,7 @@
       <c r="I106" s="2"/>
       <c r="J106" s="2"/>
     </row>
-    <row r="107" spans="1:10">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A107" s="5"/>
       <c r="B107" s="5"/>
       <c r="C107" s="2"/>
@@ -2894,7 +3269,7 @@
       <c r="I107" s="2"/>
       <c r="J107" s="2"/>
     </row>
-    <row r="108" spans="1:10">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A108" s="5"/>
       <c r="B108" s="5"/>
       <c r="C108" s="2"/>
@@ -2906,7 +3281,7 @@
       <c r="I108" s="2"/>
       <c r="J108" s="2"/>
     </row>
-    <row r="109" spans="1:10">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A109" s="5"/>
       <c r="B109" s="5"/>
       <c r="C109" s="2"/>
@@ -2918,7 +3293,7 @@
       <c r="I109" s="2"/>
       <c r="J109" s="2"/>
     </row>
-    <row r="110" spans="1:10">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A110" s="5"/>
       <c r="B110" s="5"/>
       <c r="C110" s="2"/>
@@ -2930,7 +3305,7 @@
       <c r="I110" s="2"/>
       <c r="J110" s="2"/>
     </row>
-    <row r="111" spans="1:10">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A111" s="5"/>
       <c r="B111" s="5"/>
       <c r="C111" s="2"/>
@@ -2942,7 +3317,7 @@
       <c r="I111" s="2"/>
       <c r="J111" s="2"/>
     </row>
-    <row r="112" spans="1:10">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A112" s="5"/>
       <c r="B112" s="5"/>
       <c r="C112" s="2"/>
@@ -2954,7 +3329,7 @@
       <c r="I112" s="2"/>
       <c r="J112" s="2"/>
     </row>
-    <row r="113" spans="1:10">
+    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A113" s="5"/>
       <c r="B113" s="5"/>
       <c r="C113" s="2"/>
@@ -2966,7 +3341,7 @@
       <c r="I113" s="2"/>
       <c r="J113" s="2"/>
     </row>
-    <row r="114" spans="1:10">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A114" s="5"/>
       <c r="B114" s="5"/>
       <c r="C114" s="2"/>
@@ -2978,7 +3353,7 @@
       <c r="I114" s="2"/>
       <c r="J114" s="2"/>
     </row>
-    <row r="115" spans="1:10">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A115" s="5"/>
       <c r="B115" s="5"/>
       <c r="C115" s="2"/>
@@ -2990,7 +3365,7 @@
       <c r="I115" s="2"/>
       <c r="J115" s="2"/>
     </row>
-    <row r="116" spans="1:10">
+    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A116" s="5"/>
       <c r="B116" s="5"/>
       <c r="C116" s="2"/>
@@ -3002,7 +3377,7 @@
       <c r="I116" s="2"/>
       <c r="J116" s="2"/>
     </row>
-    <row r="117" spans="1:10">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A117" s="5"/>
       <c r="B117" s="5"/>
       <c r="C117" s="2"/>
@@ -3014,7 +3389,7 @@
       <c r="I117" s="2"/>
       <c r="J117" s="2"/>
     </row>
-    <row r="118" spans="1:10">
+    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A118" s="5"/>
       <c r="B118" s="5"/>
       <c r="C118" s="2"/>
@@ -3026,7 +3401,7 @@
       <c r="I118" s="2"/>
       <c r="J118" s="2"/>
     </row>
-    <row r="119" spans="1:10">
+    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A119" s="5"/>
       <c r="B119" s="5"/>
       <c r="C119" s="2"/>
@@ -3046,16 +3421,44 @@
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
+  <oleObjects>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <oleObject progId="包装程序外壳对象" dvAspect="DVASPECT_ICON" shapeId="7" r:id="rId4">
+          <objectPr defaultSize="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>32</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>333375</xdr:colOff>
+                <xdr:row>32</xdr:row>
+                <xdr:rowOff>638175</xdr:rowOff>
+              </to>
+            </anchor>
+          </objectPr>
+        </oleObject>
+      </mc:Choice>
+      <mc:Fallback>
+        <oleObject progId="包装程序外壳对象" dvAspect="DVASPECT_ICON" shapeId="1026" r:id="rId4"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+  </oleObjects>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3063,12 +3466,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>